<commit_message>
small changes to diagram
</commit_message>
<xml_diff>
--- a/db/db_analysis/results/query_execution_times_4-7.xlsx
+++ b/db/db_analysis/results/query_execution_times_4-7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9510DDCA-4E97-2B4D-9266-DA8E665D537D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B612B080-E0C6-DB4E-8234-4D8DA6155C07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34840" yWindow="500" windowWidth="33920" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="67860" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query_execution_times_4-7" sheetId="1" r:id="rId1"/>
@@ -19,22 +19,6 @@
     <sheet name="6 tables" sheetId="4" r:id="rId4"/>
     <sheet name="7 tables" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'4 tables'!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'4 tables'!$H$2:$H$9</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'4 tables'!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'4 tables'!$H$2:$H$9</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'5 tables'!$F$2:$F$29</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'5 tables'!$H$2:$H$29</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'4 tables'!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'4 tables'!$H$2:$H$9</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'4 tables'!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'4 tables'!$H$2:$H$9</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'4 tables'!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'4 tables'!$H$2:$H$9</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'4 tables'!$F$2:$F$9</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'4 tables'!$H$2:$H$9</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
@@ -3812,9 +3796,6 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4002,13 +3983,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -4042,231 +4016,11 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -4480,9 +4234,253 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -4520,28 +4518,14 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -9855,16 +9839,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>436034</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>119239</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>131234</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>195439</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10003,7 +9987,7 @@
   <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="query hash"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="query" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="query" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="tables_involved"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="% of possible queries executed"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="n of tables"/>
@@ -10014,22 +9998,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:F29" totalsRowShown="0" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:F29" totalsRowShown="0" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="A1:F29" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="query hash" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="query" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="tables_involved" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="% of possible queries executed" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="n of tables" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="time in s" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="query hash" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="query" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="tables_involved" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="% of possible queries executed" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="n of tables" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="time in s" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A1:F61" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A1:F61" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:F61" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="query hash" dataDxfId="16"/>
@@ -10044,15 +10028,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A1:F101" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A1:F101" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="query hash" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="query" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="tables_involved" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="% of possible queries executed" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="n of tables" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="time in s" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="query hash" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="query" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="tables_involved" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="% of possible queries executed" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="n of tables" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="time in s" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14315,11 +14299,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R48" sqref="R48"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="50.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" t="s">
@@ -14566,11 +14553,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H29"/>
+    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="49.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17">
       <c r="A1" t="s">
@@ -16792,8 +16782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>